<commit_message>
Hospital Notifies patients appointments
But patients always says yes
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José\Documents\IDES\github\AIAD\AIADProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José\workspaceJava\AIADProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="5">
   <si>
     <t>livre</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>pediatria-Patient1;cardiologia-Patient3</t>
+  </si>
+  <si>
+    <t>pediatria-Patient1</t>
   </si>
 </sst>
 </file>
@@ -359,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,7 +611,7 @@
         <v>1420164000</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1277,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2195,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added utility functions on the timetable
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José\workspaceJava\AIADProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\GitHub\AIAD\AIADProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>ocupado</t>
   </si>
   <si>
-    <t>cardiologia</t>
-  </si>
-  <si>
     <t>pediatria-Patient1;cardiologia-Patient3</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>marcado</t>
+  </si>
+  <si>
+    <t>ocupador</t>
   </si>
 </sst>
 </file>
@@ -365,17 +365,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -383,7 +383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -392,7 +392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -401,7 +401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -410,7 +410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -419,7 +419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -428,7 +428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -446,7 +446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -518,7 +518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -527,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -554,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -563,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>A22+3600</f>
         <v>1420149600</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -590,34 +590,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>1420160400</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>1420164000</v>
+      </c>
+      <c r="B27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>1420160400</v>
-      </c>
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>1420164000</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -635,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -644,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -680,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -716,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -824,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -869,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -959,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -995,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -1022,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -1076,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -1184,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -1202,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -1247,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -1256,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -1283,17 +1283,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -1328,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -1346,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -1364,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -1373,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -1400,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -1409,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -1445,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -1454,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -1463,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -1472,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -1481,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -1490,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -1508,232 +1508,232 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>1420160400</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>1420164000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>1420167600</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>1420171200</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>1420174800</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>1420178400</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>1420182000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>1420185600</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>1420189200</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>1420192800</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>1420196400</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>1420200000</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>1420203600</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>1420207200</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>1420210800</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>1420214400</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>1420218000</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>1420221600</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>1420225200</v>
+      </c>
+      <c r="B44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>1420160400</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>1420164000</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>1420167600</v>
-      </c>
-      <c r="B28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>1420171200</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>1420174800</v>
-      </c>
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>1420178400</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>1420182000</v>
-      </c>
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>1420185600</v>
-      </c>
-      <c r="B33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>1420189200</v>
-      </c>
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>1420192800</v>
-      </c>
-      <c r="B35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>1420196400</v>
-      </c>
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>1420200000</v>
-      </c>
-      <c r="B37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>1420203600</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>1420207200</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>1420210800</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>1420214400</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>1420218000</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>1420221600</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>1420225200</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
       </c>
       <c r="B49" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -1751,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -1760,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -1787,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -1814,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -1850,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -1895,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -1922,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -1931,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -1940,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -1958,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -1985,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -2003,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -2012,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -2021,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -2030,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -2039,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -2066,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -2084,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -2093,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -2102,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -2138,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -2174,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -2201,17 +2201,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -2228,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -2273,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -2282,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -2291,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -2300,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -2354,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -2363,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -2372,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -2381,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -2390,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -2399,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -2408,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
@@ -2417,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -2426,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -2462,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -2471,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -2498,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -2534,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -2561,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -2579,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -2597,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -2606,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -2615,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -2624,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -2633,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -2651,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -2669,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -2678,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -2696,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -2732,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -2750,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -2759,7 +2759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -2777,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -2786,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -2795,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -2849,7 +2849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -2858,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -2867,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -2876,7 +2876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -2903,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -2921,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -2930,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -2948,7 +2948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -2957,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -2966,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -2993,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -3011,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -3020,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -3029,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -3038,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -3056,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -3065,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -3074,7 +3074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -3083,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -3092,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -3101,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -3119,17 +3119,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -3146,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -3155,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -3164,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -3173,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -3191,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -3200,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -3209,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -3218,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -3227,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -3245,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -3254,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -3263,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -3281,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -3290,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -3299,7 +3299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -3308,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -3317,7 +3317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -3326,16 +3326,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -3344,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -3362,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -3371,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -3398,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -3407,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -3425,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -3443,7 +3443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -3461,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -3470,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -3479,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -3488,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -3497,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -3506,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -3515,7 +3515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -3524,7 +3524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -3533,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -3542,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -3551,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -3560,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -3569,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -3578,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -3587,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -3596,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -3605,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -3623,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -3641,7 +3641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -3650,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -3659,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -3668,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -3677,7 +3677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -3686,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -3695,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -3704,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -3713,7 +3713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -3722,7 +3722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -3731,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -3740,7 +3740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -3749,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -3758,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -3767,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -3776,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -3785,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -3803,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -3812,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -3830,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -3839,7 +3839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -3848,7 +3848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -3857,7 +3857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -3866,7 +3866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -3875,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -3884,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -3893,7 +3893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -3902,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -3911,7 +3911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -3920,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -3929,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -3938,7 +3938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -3947,7 +3947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -3956,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -3974,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -3983,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -3992,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -4001,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -4010,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -4019,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -4037,17 +4037,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -4064,7 +4064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -4073,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -4082,7 +4082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -4091,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -4100,7 +4100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -4109,7 +4109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -4118,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -4127,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -4136,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -4145,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -4154,7 +4154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -4163,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -4172,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -4181,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -4190,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -4199,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -4208,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -4226,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -4235,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
@@ -4253,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
@@ -4271,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -4280,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -4289,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -4307,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -4316,7 +4316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -4325,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -4334,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -4343,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -4352,7 +4352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -4361,7 +4361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -4370,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -4379,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -4388,7 +4388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -4397,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -4406,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -4415,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -4424,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -4433,7 +4433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -4442,7 +4442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -4451,7 +4451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -4460,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -4469,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -4478,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -4487,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -4496,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -4505,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -4514,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -4523,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -4532,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -4541,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -4550,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -4559,7 +4559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -4568,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -4577,7 +4577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -4586,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -4595,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -4604,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -4613,7 +4613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -4622,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -4631,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -4640,7 +4640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -4649,7 +4649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -4658,7 +4658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -4667,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -4676,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -4685,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -4694,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -4703,7 +4703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -4712,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -4730,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -4748,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -4766,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -4775,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -4784,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -4793,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -4802,7 +4802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -4811,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -4820,7 +4820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -4829,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -4838,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -4856,7 +4856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -4865,7 +4865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -4874,7 +4874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -4883,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -4892,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -4901,7 +4901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -4910,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -4919,7 +4919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -4928,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -4937,7 +4937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>

</xml_diff>

<commit_message>
hospital planner closes at night
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="5">
   <si>
     <t>livre</t>
   </si>
@@ -36,16 +36,13 @@
     <t>ocupado</t>
   </si>
   <si>
-    <t>pediatria-Patient1;cardiologia-Patient3</t>
-  </si>
-  <si>
-    <t>pediatria-Patient1</t>
-  </si>
-  <si>
     <t>marcado</t>
   </si>
   <si>
     <t>ocupador</t>
+  </si>
+  <si>
+    <t>fechado</t>
   </si>
 </sst>
 </file>
@@ -365,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J104" sqref="J104"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,7 +377,7 @@
         <v>1420070400</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -389,7 +386,7 @@
         <v>1420074000</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,7 +395,7 @@
         <v>1420077600</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -407,7 +404,7 @@
         <v>1420081200</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -416,7 +413,7 @@
         <v>1420084800</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -425,7 +422,7 @@
         <v>1420088400</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,7 +431,7 @@
         <v>1420092000</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,7 +440,7 @@
         <v>1420095600</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +449,7 @@
         <v>1420099200</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +566,7 @@
         <v>1420146000</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -578,7 +575,7 @@
         <v>1420149600</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -587,7 +584,7 @@
         <v>1420153200</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +593,7 @@
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +602,7 @@
         <v>1420160400</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -614,7 +611,7 @@
         <v>1420164000</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -623,7 +620,7 @@
         <v>1420167600</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -632,7 +629,7 @@
         <v>1420171200</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +638,7 @@
         <v>1420174800</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,7 +647,7 @@
         <v>1420178400</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +656,7 @@
         <v>1420182000</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +665,7 @@
         <v>1420185600</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +674,7 @@
         <v>1420189200</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +791,7 @@
         <v>1420236000</v>
       </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +800,7 @@
         <v>1420239600</v>
       </c>
       <c r="B48" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +809,7 @@
         <v>1420243200</v>
       </c>
       <c r="B49" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -821,7 +818,7 @@
         <v>1420246800</v>
       </c>
       <c r="B50" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +827,7 @@
         <v>1420250400</v>
       </c>
       <c r="B51" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +836,7 @@
         <v>1420254000</v>
       </c>
       <c r="B52" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +845,7 @@
         <v>1420257600</v>
       </c>
       <c r="B53" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
         <v>1420261200</v>
       </c>
       <c r="B54" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,7 +863,7 @@
         <v>1420264800</v>
       </c>
       <c r="B55" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +872,7 @@
         <v>1420268400</v>
       </c>
       <c r="B56" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -884,7 +881,7 @@
         <v>1420272000</v>
       </c>
       <c r="B57" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -893,7 +890,7 @@
         <v>1420275600</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +899,7 @@
         <v>1420279200</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +1016,7 @@
         <v>1420326000</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1028,7 +1025,7 @@
         <v>1420329600</v>
       </c>
       <c r="B73" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1037,7 +1034,7 @@
         <v>1420333200</v>
       </c>
       <c r="B74" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1043,7 @@
         <v>1420336800</v>
       </c>
       <c r="B75" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,7 +1052,7 @@
         <v>1420340400</v>
       </c>
       <c r="B76" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,7 +1061,7 @@
         <v>1420344000</v>
       </c>
       <c r="B77" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1073,7 +1070,7 @@
         <v>1420347600</v>
       </c>
       <c r="B78" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1082,7 +1079,7 @@
         <v>1420351200</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1091,7 +1088,7 @@
         <v>1420354800</v>
       </c>
       <c r="B80" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1100,7 +1097,7 @@
         <v>1420358400</v>
       </c>
       <c r="B81" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,7 +1106,7 @@
         <v>1420362000</v>
       </c>
       <c r="B82" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1118,7 +1115,7 @@
         <v>1420365600</v>
       </c>
       <c r="B83" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1241,7 @@
         <v>1420416000</v>
       </c>
       <c r="B97" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,7 +1250,7 @@
         <v>1420419600</v>
       </c>
       <c r="B98" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
         <v>1420423200</v>
       </c>
       <c r="B99" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,7 +1268,7 @@
         <v>1420426800</v>
       </c>
       <c r="B100" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1514,7 +1511,7 @@
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,7 +1682,7 @@
         <v>1420225200</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1694,7 +1691,7 @@
         <v>1420228800</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1703,7 +1700,7 @@
         <v>1420232400</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1712,7 +1709,7 @@
         <v>1420236000</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1721,7 +1718,7 @@
         <v>1420239600</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1730,7 +1727,7 @@
         <v>1420243200</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3332,7 +3329,7 @@
         <v>1420149600</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
created function to cancel sonsultations
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -362,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2ºalgoritmo de marcacao acrescentado
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\GitHub\AIAD\AIADProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José\workspaceJava\AIADProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Hospital" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="3">
   <si>
     <t>livre</t>
   </si>
   <si>
     <t>ocupado</t>
-  </si>
-  <si>
-    <t>marcado</t>
-  </si>
-  <si>
-    <t>ocupador</t>
   </si>
   <si>
     <t>fechado</t>
@@ -362,97 +356,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1420070400</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -461,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -470,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -479,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -488,16 +482,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -506,7 +500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -515,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -524,7 +518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -533,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -542,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -551,133 +545,133 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>A22+3600</f>
         <v>1420149600</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -686,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -695,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -704,16 +698,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
       </c>
       <c r="B38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -722,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -731,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -740,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -749,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -758,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -767,142 +761,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
       </c>
       <c r="B45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
       </c>
       <c r="B46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -911,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -920,16 +914,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
       </c>
       <c r="B62" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -938,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -947,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -956,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -965,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -974,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -983,142 +977,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
       </c>
       <c r="B69" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
       </c>
       <c r="B70" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
       </c>
       <c r="B71" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -1127,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -1136,16 +1130,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -1154,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -1163,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -1172,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -1181,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -1190,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -1199,76 +1193,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
       </c>
       <c r="B93" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
       </c>
       <c r="B94" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
       </c>
       <c r="B95" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
       </c>
       <c r="B96" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1281,16 +1275,16 @@
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -1298,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -1307,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -1316,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -1325,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -1334,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -1343,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -1352,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -1361,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -1370,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -1379,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -1388,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -1397,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -1406,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -1415,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -1424,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -1433,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -1442,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -1451,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -1460,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -1469,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -1478,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -1487,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
@@ -1496,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -1505,16 +1499,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -1523,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -1532,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -1541,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -1550,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -1559,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -1568,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -1577,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -1586,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -1595,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -1604,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -1613,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -1622,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -1631,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -1640,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -1649,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -1658,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -1667,7 +1661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -1676,61 +1670,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -1739,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -1748,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -1757,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -1766,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -1775,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -1784,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -1793,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -1802,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -1811,16 +1805,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -1829,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -1838,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -1847,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -1856,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -1865,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -1874,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -1883,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -1892,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -1901,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -1910,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -1919,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -1928,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -1937,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -1946,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -1955,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -1964,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -1973,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -1982,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -1991,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -2000,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -2009,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -2018,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -2027,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -2036,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -2045,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -2054,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -2063,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -2072,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -2081,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -2090,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -2099,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -2108,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -2117,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -2126,7 +2120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -2135,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -2144,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -2153,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -2162,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -2171,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -2180,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -2198,17 +2192,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -2216,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -2225,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -2234,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -2243,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -2252,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -2261,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -2270,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -2279,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -2288,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -2297,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -2306,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -2315,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -2324,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -2333,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -2342,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -2351,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -2360,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -2369,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -2378,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -2387,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -2396,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -2405,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
@@ -2414,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -2423,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
@@ -2432,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -2441,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -2450,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -2459,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -2468,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -2477,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -2486,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -2495,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -2504,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -2513,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -2522,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -2531,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -2540,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -2549,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -2558,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -2567,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -2576,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -2585,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -2594,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -2603,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -2612,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -2621,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -2630,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -2639,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -2648,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -2657,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -2666,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -2675,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -2684,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -2693,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -2702,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -2711,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -2720,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -2729,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -2738,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -2747,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -2756,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -2765,7 +2759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -2774,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -2783,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -2792,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -2801,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -2810,7 +2804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -2819,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -2828,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -2837,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -2846,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -2855,7 +2849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -2864,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -2873,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -2882,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -2891,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -2900,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -2909,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -2918,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -2927,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -2936,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -2945,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -2954,7 +2948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -2963,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -2972,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -2981,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -2990,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -2999,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -3008,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -3017,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -3026,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -3035,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -3044,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -3053,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -3062,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -3071,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -3080,7 +3074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -3089,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -3098,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -3116,17 +3110,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D24"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -3134,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -3143,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -3152,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -3161,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -3170,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -3179,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -3188,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -3197,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -3206,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -3215,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -3224,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -3233,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -3242,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -3251,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -3260,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -3269,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -3278,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -3287,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -3296,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -3305,7 +3299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -3314,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -3323,16 +3317,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -3341,16 +3335,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -3359,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -3368,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -3377,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -3386,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -3395,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -3404,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -3413,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -3422,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -3431,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -3440,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -3449,7 +3443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -3458,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -3467,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -3476,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -3485,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -3494,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -3503,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -3512,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -3521,7 +3515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -3530,7 +3524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -3539,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -3548,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -3557,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -3566,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -3575,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -3584,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -3593,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -3602,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -3611,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -3620,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -3629,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -3638,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -3647,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -3656,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -3665,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -3674,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -3683,7 +3677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -3692,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -3701,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -3710,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -3719,7 +3713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -3728,7 +3722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -3737,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -3746,7 +3740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -3755,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -3764,7 +3758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -3773,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -3782,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -3791,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -3800,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -3809,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -3818,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -3827,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -3836,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -3845,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -3854,7 +3848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -3863,7 +3857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -3872,7 +3866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -3881,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -3890,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -3899,7 +3893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -3908,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -3917,7 +3911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -3926,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -3935,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -3944,7 +3938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -3953,7 +3947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -3962,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -3971,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -3980,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -3989,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -3998,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -4007,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -4016,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>
@@ -4034,17 +4028,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1420070400</v>
       </c>
@@ -4052,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>A1+3600</f>
         <v>1420074000</v>
@@ -4061,7 +4055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">A2+3600</f>
         <v>1420077600</v>
@@ -4070,7 +4064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1420081200</v>
@@ -4079,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1420084800</v>
@@ -4088,7 +4082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1420088400</v>
@@ -4097,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1420092000</v>
@@ -4106,7 +4100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1420095600</v>
@@ -4115,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1420099200</v>
@@ -4124,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1420102800</v>
@@ -4133,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1420106400</v>
@@ -4142,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1420110000</v>
@@ -4151,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1420113600</v>
@@ -4160,7 +4154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1420117200</v>
@@ -4169,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1420120800</v>
@@ -4178,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1420124400</v>
@@ -4187,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1420128000</v>
@@ -4196,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1420131600</v>
@@ -4205,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1420135200</v>
@@ -4214,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1420138800</v>
@@ -4223,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1420142400</v>
@@ -4232,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1420146000</v>
@@ -4241,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1420149600</v>
@@ -4250,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1420153200</v>
@@ -4259,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1420156800</v>
@@ -4268,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1420160400</v>
@@ -4277,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1420164000</v>
@@ -4286,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1420167600</v>
@@ -4295,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1420171200</v>
@@ -4304,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1420174800</v>
@@ -4313,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1420178400</v>
@@ -4322,7 +4316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1420182000</v>
@@ -4331,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1420185600</v>
@@ -4340,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1420189200</v>
@@ -4349,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1420192800</v>
@@ -4358,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1420196400</v>
@@ -4367,7 +4361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>1420200000</v>
@@ -4376,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>1420203600</v>
@@ -4385,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>1420207200</v>
@@ -4394,7 +4388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>1420210800</v>
@@ -4403,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>1420214400</v>
@@ -4412,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>1420218000</v>
@@ -4421,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>1420221600</v>
@@ -4430,7 +4424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>1420225200</v>
@@ -4439,7 +4433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>1420228800</v>
@@ -4448,7 +4442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>1420232400</v>
@@ -4457,7 +4451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>1420236000</v>
@@ -4466,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>1420239600</v>
@@ -4475,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>1420243200</v>
@@ -4484,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>1420246800</v>
@@ -4493,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>1420250400</v>
@@ -4502,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>1420254000</v>
@@ -4511,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>1420257600</v>
@@ -4520,7 +4514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>1420261200</v>
@@ -4529,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>1420264800</v>
@@ -4538,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>1420268400</v>
@@ -4547,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>1420272000</v>
@@ -4556,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>1420275600</v>
@@ -4565,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>1420279200</v>
@@ -4574,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>1420282800</v>
@@ -4583,7 +4577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>1420286400</v>
@@ -4592,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>1420290000</v>
@@ -4601,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>1420293600</v>
@@ -4610,7 +4604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>1420297200</v>
@@ -4619,7 +4613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1420300800</v>
@@ -4628,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1420304400</v>
@@ -4637,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+3600</f>
         <v>1420308000</v>
@@ -4646,7 +4640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1420311600</v>
@@ -4655,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1420315200</v>
@@ -4664,7 +4658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1420318800</v>
@@ -4673,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1420322400</v>
@@ -4682,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1420326000</v>
@@ -4691,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1420329600</v>
@@ -4700,7 +4694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1420333200</v>
@@ -4709,7 +4703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1420336800</v>
@@ -4718,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1420340400</v>
@@ -4727,7 +4721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1420344000</v>
@@ -4736,7 +4730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1420347600</v>
@@ -4745,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1420351200</v>
@@ -4754,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1420354800</v>
@@ -4763,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1420358400</v>
@@ -4772,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1420362000</v>
@@ -4781,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1420365600</v>
@@ -4790,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1420369200</v>
@@ -4799,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1420372800</v>
@@ -4808,7 +4802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1420376400</v>
@@ -4817,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1420380000</v>
@@ -4826,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1420383600</v>
@@ -4835,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1420387200</v>
@@ -4844,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1420390800</v>
@@ -4853,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1420394400</v>
@@ -4862,7 +4856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1420398000</v>
@@ -4871,7 +4865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1420401600</v>
@@ -4880,7 +4874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1420405200</v>
@@ -4889,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1420408800</v>
@@ -4898,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1420412400</v>
@@ -4907,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>1420416000</v>
@@ -4916,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1420419600</v>
@@ -4925,7 +4919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1420423200</v>
@@ -4934,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1420426800</v>

</xml_diff>

<commit_message>
Reappointments done and...code reorganized in patient
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="5">
   <si>
     <t>livre</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>fechado</t>
+  </si>
+  <si>
+    <t>pediatria-Patient1</t>
+  </si>
+  <si>
+    <t>pediatria-Patient3</t>
   </si>
 </sst>
 </file>
@@ -356,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +737,7 @@
         <v>1420214400</v>
       </c>
       <c r="B41" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -758,7 +764,7 @@
         <v>1420225200</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1274,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2192,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3110,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3485,7 +3491,7 @@
         <v>1420214400</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -3521,7 +3527,7 @@
         <v>1420228800</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
bugs in algorith appointment correted
</commit_message>
<xml_diff>
--- a/AIADProject/TimeTable.xlsx
+++ b/AIADProject/TimeTable.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="3">
   <si>
     <t>livre</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>fechado</t>
-  </si>
-  <si>
-    <t>pediatria-Patient1</t>
-  </si>
-  <si>
-    <t>pediatria-Patient3</t>
   </si>
 </sst>
 </file>
@@ -737,7 +731,7 @@
         <v>1420214400</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -764,7 +758,7 @@
         <v>1420225200</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>